<commit_message>
add support for logInTest from data provided by excel
</commit_message>
<xml_diff>
--- a/src/test/resources/testData.xlsx
+++ b/src/test/resources/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JavaProgramowanie\Nauka\seleniumtests\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF20EDF-E167-4B68-AD93-D7B6120140F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5F0ED4-4914-4613-8FE8-185A28BF1594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3888" yWindow="1596" windowWidth="17280" windowHeight="8976" xr2:uid="{C306C8A3-0080-41EE-9645-ADC12B967724}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8976" xr2:uid="{C306C8A3-0080-41EE-9645-ADC12B967724}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -44,6 +44,15 @@
     <t>email</t>
   </si>
   <si>
+    <t>tst111@test.com</t>
+  </si>
+  <si>
+    <t>tst222@test.com</t>
+  </si>
+  <si>
+    <t>tst333@test.com</t>
+  </si>
+  <si>
     <t>password</t>
   </si>
   <si>
@@ -74,64 +83,55 @@
     <t>order_notes(opt)</t>
   </si>
   <si>
-    <t>tst111@test.com</t>
-  </si>
-  <si>
-    <t>tst222@test.com</t>
-  </si>
-  <si>
-    <t>tst333@test.com</t>
-  </si>
-  <si>
     <t>SecurePassw1!</t>
   </si>
   <si>
+    <t>Name1</t>
+  </si>
+  <si>
+    <t>Surname1</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>Address 1 22-333 4/5</t>
+  </si>
+  <si>
+    <t>City1</t>
+  </si>
+  <si>
     <t>SecurePassw2!</t>
   </si>
   <si>
+    <t>Name2</t>
+  </si>
+  <si>
+    <t>Surname2</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>City2</t>
+  </si>
+  <si>
     <t>SecurePassw3!</t>
   </si>
   <si>
-    <t>Name1</t>
-  </si>
-  <si>
-    <t>Name2</t>
-  </si>
-  <si>
     <t>Name3</t>
   </si>
   <si>
-    <t>Surname1</t>
-  </si>
-  <si>
-    <t>Surname2</t>
-  </si>
-  <si>
     <t>Surname3</t>
   </si>
   <si>
-    <t>Finland</t>
-  </si>
-  <si>
-    <t>Germany</t>
-  </si>
-  <si>
     <t>Poland</t>
   </si>
   <si>
-    <t>Address 1 22-333 4/5</t>
-  </si>
-  <si>
-    <t>City1</t>
-  </si>
-  <si>
-    <t>City2</t>
+    <t>22-222</t>
   </si>
   <si>
     <t>City3</t>
-  </si>
-  <si>
-    <t>22-222</t>
   </si>
   <si>
     <t>123456789</t>
@@ -178,10 +178,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -519,170 +517,158 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="1"/>
-    <col min="8" max="8" width="18.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.88671875" style="1"/>
-    <col min="11" max="11" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="I1" t="s">
         <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="2">
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2">
         <v>323123</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" s="2">
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2">
         <v>123456789</v>
       </c>
-      <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2" t="s">
+      <c r="I3">
+        <v>546454</v>
+      </c>
+      <c r="J3" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="2">
-        <v>546454</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" s="2">
+      <c r="K3">
         <v>123456789</v>
       </c>
-      <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="D4" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="K4" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add dataprovider to PurchaseTest
</commit_message>
<xml_diff>
--- a/src/test/resources/testData.xlsx
+++ b/src/test/resources/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JavaProgramowanie\Nauka\seleniumtests\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5F0ED4-4914-4613-8FE8-185A28BF1594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F055681-3FE7-40DE-BA0B-82ACDEC55941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8976" xr2:uid="{C306C8A3-0080-41EE-9645-ADC12B967724}"/>
+    <workbookView xWindow="2400" yWindow="1116" windowWidth="17280" windowHeight="8976" xr2:uid="{C306C8A3-0080-41EE-9645-ADC12B967724}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
-  <si>
-    <t>id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>email</t>
   </si>
@@ -125,16 +122,10 @@
     <t>Surname3</t>
   </si>
   <si>
-    <t>Poland</t>
-  </si>
-  <si>
-    <t>22-222</t>
-  </si>
-  <si>
     <t>City3</t>
   </si>
   <si>
-    <t>123456789</t>
+    <t>France</t>
   </si>
 </sst>
 </file>
@@ -178,8 +169,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -514,31 +506,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E0AC967-CB6E-431A-A0A9-0C8B7AF89C1D}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -567,16 +558,13 @@
       <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -584,31 +572,28 @@
       <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>17</v>
       </c>
       <c r="G2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2">
+        <v>32323</v>
+      </c>
+      <c r="I2" t="s">
         <v>19</v>
       </c>
-      <c r="I2">
-        <v>323123</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="J2">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>20</v>
-      </c>
-      <c r="K2">
-        <v>123456789</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -616,31 +601,28 @@
       <c r="D3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>23</v>
       </c>
       <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <v>54645</v>
+      </c>
+      <c r="I3" t="s">
         <v>24</v>
       </c>
-      <c r="H3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3">
-        <v>546454</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="J3">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>25</v>
-      </c>
-      <c r="K3">
-        <v>123456789</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
       </c>
       <c r="C4" t="s">
         <v>26</v>
@@ -648,23 +630,20 @@
       <c r="D4" t="s">
         <v>27</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4">
+        <v>70003</v>
+      </c>
+      <c r="I4" t="s">
         <v>28</v>
       </c>
-      <c r="G4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" t="s">
-        <v>32</v>
+      <c r="J4" s="1">
+        <v>123456789</v>
       </c>
     </row>
   </sheetData>

</xml_diff>